<commit_message>
Excel with score formulas
</commit_message>
<xml_diff>
--- a/FruitGame_FGJ2014.xlsx
+++ b/FruitGame_FGJ2014.xlsx
@@ -12,16 +12,17 @@
     <sheet name="aggroTable" sheetId="5" r:id="rId3"/>
     <sheet name="greatPersonSpawning" sheetId="6" r:id="rId4"/>
     <sheet name="fruitSpawning" sheetId="7" r:id="rId5"/>
-    <sheet name="flow" sheetId="4" r:id="rId6"/>
-    <sheet name="test" sheetId="3" r:id="rId7"/>
-    <sheet name="Taul1" sheetId="1" r:id="rId8"/>
+    <sheet name="score" sheetId="10" r:id="rId6"/>
+    <sheet name="flow" sheetId="4" r:id="rId7"/>
+    <sheet name="test" sheetId="3" r:id="rId8"/>
+    <sheet name="Taul1" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="211">
   <si>
     <t>hyljeksimisprosentti</t>
   </si>
@@ -568,6 +569,93 @@
   <si>
     <t>Down%</t>
   </si>
+  <si>
+    <t>rand 20</t>
+  </si>
+  <si>
+    <t>vendettaConstant</t>
+  </si>
+  <si>
+    <t>vendettaBaseMultiplier</t>
+  </si>
+  <si>
+    <t>vendettaRadius</t>
+  </si>
+  <si>
+    <t>fruitSpawnController</t>
+  </si>
+  <si>
+    <t>fruitSpawnChance</t>
+  </si>
+  <si>
+    <t>ome</t>
+  </si>
+  <si>
+    <t>pää</t>
+  </si>
+  <si>
+    <t>ban</t>
+  </si>
+  <si>
+    <t>ryp</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>1 = ome</t>
+  </si>
+  <si>
+    <t>2 = ban</t>
+  </si>
+  <si>
+    <t>3 = ryp</t>
+  </si>
+  <si>
+    <t>4 = pää</t>
+  </si>
+  <si>
+    <t>1 = pun</t>
+  </si>
+  <si>
+    <t>2 = sin</t>
+  </si>
+  <si>
+    <t>3 = vih</t>
+  </si>
+  <si>
+    <t>4 = kel</t>
+  </si>
+  <si>
+    <t>ka</t>
+  </si>
+  <si>
+    <t>diversity</t>
+  </si>
+  <si>
+    <t>SCORE</t>
+  </si>
+  <si>
+    <t>base diversity score</t>
+  </si>
+  <si>
+    <t>full unity</t>
+  </si>
+  <si>
+    <t>1 nation</t>
+  </si>
+  <si>
+    <t>1 belief</t>
+  </si>
+  <si>
+    <t>SCORE TOTAL</t>
+  </si>
+  <si>
+    <t>populationBalancer</t>
+  </si>
+  <si>
+    <t>populationMultiplier</t>
+  </si>
 </sst>
 </file>
 
@@ -606,7 +694,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -723,11 +811,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -743,6 +840,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,10 +1027,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.005882352941182</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.864705882352951</c:v>
+                  <c:v>25.305882352941179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -946,11 +1046,11 @@
         </c:dLbls>
         <c:gapWidth val="160"/>
         <c:overlap val="-10"/>
-        <c:axId val="120058624"/>
-        <c:axId val="120060160"/>
+        <c:axId val="121565952"/>
+        <c:axId val="121567488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="120058624"/>
+        <c:axId val="121565952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -959,7 +1059,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120060160"/>
+        <c:crossAx val="121567488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -967,7 +1067,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120060160"/>
+        <c:axId val="121567488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -980,7 +1080,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120058624"/>
+        <c:crossAx val="121565952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1018,11 +1118,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="$W$5" horiz="1" max="25" page="10" val="18"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="$W$5" horiz="1" max="25" page="10" val="19"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="$W$6" horiz="1" max="25" page="10" val="7"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="$W$6" horiz="1" max="25" page="10" val="11"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3696,6 +3796,1084 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rounded Rectangle 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9515475" y="381000"/>
+          <a:ext cx="4114800" cy="2476500"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>GOAL</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> 1: LET ALL THE FLOWERS BLOOM</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t>Aim for ultimate diversity: equal amounts of all fruits and ideals.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fi-FI" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t>((diversityBaseScore - (amountOmena - kansat.Keskiarvo)) +</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(diversityBaseScore - (amountBanaani - kansat.Keskiarvo)) +</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(diversityBaseScore - (amountRypale - kansat.Keskiarvo)) +</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(diversityBaseScore - (amountPaaryna - kansat.Keskiarvo)) +</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(diversityBaseScore - (amountPunainen - aatteet.Keskiarvo)) +</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(diversityBaseScore - (amountSininen - aatteet.Keskiarvo)) +</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(diversityBaseScore - (amountVihrea - aatteet.Keskiarvo)) +</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(diversityBaseScore - (amountKeltainen - aatteet.Keskiarvo))) *</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>populationMultiplier</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rounded Rectangle 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9515475" y="3048000"/>
+          <a:ext cx="4114800" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>GOAL</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> 2: UNITED PEOPLE, FREE THINKING</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t>Aim for one great fruit people with equal ideals.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fi-FI" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(largestNationCount +</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(diversityBaseScore - (amountPunainen - aatteet.Keskiarvo)) +</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(diversityBaseScore - (amountSininen - aatteet.Keskiarvo)) +</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(diversityBaseScore - (amountVihrea - aatteet.Keskiarvo)) +</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(diversityBaseScore - (amountKeltainen - aatteet.Keskiarvo))</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>* populationMultiplier</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rounded Rectangle 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9515475" y="5143500"/>
+          <a:ext cx="4114800" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>GOAL</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> 3: HEGEMONY</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t>Unite all different fruits under one ideal.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fi-FI" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t>(largestIdealCount +</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t>(diversityBaseScore - (amountOmena - kansat.Keskiarvo)) +</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(diversityBaseScore - (amountBanaani - kansat.Keskiarvo)) +</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(diversityBaseScore - (amountRypale - kansat.Keskiarvo)) +</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(diversityBaseScore - (amountPaaryna - kansat.Keskiarvo))) *</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>populationMultiplier</a:t>
+          </a:r>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rounded Rectangle 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9515475" y="7239000"/>
+          <a:ext cx="4114800" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100"/>
+            <a:t>GOAL</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t> 4: THERE CAN BE ONLY ONE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1100" baseline="0"/>
+            <a:t>Aim for one fruit people with one ideal.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fi-FI" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fi-FI">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>highestComboCount * population Multiplier</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fi-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -5433,10 +6611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AH25"/>
+  <dimension ref="B2:AH38"/>
   <sheetViews>
-    <sheetView topLeftCell="K25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5530,7 +6708,7 @@
       </c>
       <c r="AA3">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AB3">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -5538,7 +6716,7 @@
       </c>
       <c r="AC3">
         <f ca="1">RANDBETWEEN(1, 100)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:34" x14ac:dyDescent="0.25">
@@ -5607,7 +6785,7 @@
       </c>
       <c r="AC4">
         <f ca="1">RANDBETWEEN(1, 100)</f>
-        <v>99</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="2:34" x14ac:dyDescent="0.25">
@@ -5675,7 +6853,7 @@
       </c>
       <c r="AC5">
         <f ca="1">RANDBETWEEN(1, 100)</f>
-        <v>2</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:34" x14ac:dyDescent="0.25">
@@ -6513,6 +7691,46 @@
       </c>
       <c r="Q25">
         <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>183</v>
+      </c>
+      <c r="E33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>184</v>
+      </c>
+      <c r="E34">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>185</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>186</v>
+      </c>
+      <c r="E37">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>187</v>
+      </c>
+      <c r="E38">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -6561,7 +7779,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6724,11 +7944,11 @@
         <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <f>INDEX(Table2[aate], MATCH($B$4, Table2[Entiteetti], 0))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <f>INDEX(Table2[kansa], MATCH($B$4, Table2[Entiteetti], 0))</f>
@@ -6748,15 +7968,15 @@
       </c>
       <c r="H4">
         <f>INDEX(Table2[vihr%], MATCH($B$4, Table2[Entiteetti], 0))</f>
-        <v>20</v>
+        <v>11.25</v>
       </c>
       <c r="I4">
         <f>INDEX(Table2[pun%], MATCH($B$4, Table2[Entiteetti], 0))</f>
-        <v>20</v>
+        <v>11.25</v>
       </c>
       <c r="J4">
         <f>INDEX(Table2[sin%], MATCH($B$4, Table2[Entiteetti], 0))</f>
-        <v>20</v>
+        <v>11.25</v>
       </c>
       <c r="K4">
         <f>INDEX(Table2[kelt%], MATCH($B$4, Table2[Entiteetti], 0))</f>
@@ -6784,23 +8004,23 @@
       </c>
       <c r="Q4">
         <f>INDEX(Table2[krtMuu], MATCH($B$4, Table2[Entiteetti], 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4">
         <f ca="1">IF(U8 = 1, 5, 0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W4">
         <f>H4*$T$1</f>
-        <v>22</v>
+        <v>12.375000000000002</v>
       </c>
       <c r="X4">
         <f t="shared" ref="X4:Z4" si="0">I4*$T$1</f>
-        <v>22</v>
+        <v>12.375000000000002</v>
       </c>
       <c r="Y4">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>12.375000000000002</v>
       </c>
       <c r="Z4">
         <f t="shared" si="0"/>
@@ -6808,27 +8028,27 @@
       </c>
       <c r="AA4">
         <f>H4*$T$2</f>
-        <v>15</v>
+        <v>8.4375</v>
       </c>
       <c r="AB4">
         <f t="shared" ref="AB4:AD4" si="1">I4*$T$2</f>
-        <v>15</v>
+        <v>8.4375</v>
       </c>
       <c r="AC4">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>8.4375</v>
       </c>
       <c r="AD4">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" t="e">
         <f>L4+V8</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AF4">
         <f t="shared" ref="AF4:AH4" ca="1" si="2">M4+W8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4">
         <f t="shared" ca="1" si="2"/>
@@ -6860,11 +8080,11 @@
         <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="C5">
         <f>INDEX(Table2[aate], MATCH($B$5, Table2[Entiteetti], 0))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <f>INDEX(Table2[kansa], MATCH($B$4, Table2[Entiteetti], 0))</f>
@@ -6884,15 +8104,15 @@
       </c>
       <c r="H5">
         <f>INDEX(Table2[vihr%], MATCH($B$5, Table2[Entiteetti], 0))</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I5">
         <f>INDEX(Table2[pun%], MATCH($B$5, Table2[Entiteetti], 0))</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J5">
         <f>INDEX(Table2[sin%], MATCH($B$5, Table2[Entiteetti], 0))</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K5">
         <f>INDEX(Table2[kelt%], MATCH($B$5, Table2[Entiteetti], 0))</f>
@@ -6919,24 +8139,24 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <f>INDEX(Table2[krtMuu], MATCH($B$4, Table2[Entiteetti], 0))</f>
+        <f>INDEX(Table2[krtMuu], MATCH($B$5, Table2[Entiteetti], 0))</f>
         <v>1</v>
       </c>
       <c r="S5">
         <f ca="1">IF(U8=1, C4, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W5">
         <f>H5*$T$1</f>
-        <v>22</v>
+        <v>16.5</v>
       </c>
       <c r="X5">
         <f t="shared" ref="X5" si="4">I5*$T$1</f>
-        <v>22</v>
+        <v>16.5</v>
       </c>
       <c r="Y5">
         <f>J5*$T$1</f>
-        <v>22</v>
+        <v>16.5</v>
       </c>
       <c r="Z5">
         <f t="shared" ref="Z5" si="5">K5*$T$1</f>
@@ -6944,15 +8164,15 @@
       </c>
       <c r="AA5">
         <f>H5*$T$2</f>
-        <v>15</v>
+        <v>11.25</v>
       </c>
       <c r="AB5">
         <f t="shared" ref="AB5" si="6">I5*$T$2</f>
-        <v>15</v>
+        <v>11.25</v>
       </c>
       <c r="AC5">
         <f t="shared" ref="AC5" si="7">J5*$T$2</f>
-        <v>15</v>
+        <v>11.25</v>
       </c>
       <c r="AD5">
         <f>K5*$T$2</f>
@@ -6964,7 +8184,7 @@
       </c>
       <c r="AF5">
         <f ca="1">M5+W9</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG5">
         <f t="shared" ref="AG5" ca="1" si="8">N5+X9</f>
@@ -7132,13 +8352,13 @@
         <v>10</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H8">
         <v>20</v>
       </c>
       <c r="I8">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J8">
         <v>20</v>
@@ -7159,7 +8379,7 @@
         <v>0</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8">
         <v>1</v>
@@ -7170,19 +8390,19 @@
       </c>
       <c r="T8">
         <f>IF(C4=C5, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8">
         <f ca="1">IF((U9-G4) &lt; AA8, 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="V8" t="e">
         <f>((1-(ABS(P4-Q4)))/(P4+Q4) * ((P4+Q4)/2))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="W8">
         <f ca="1">IF($W$10 &lt; AD8, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X8">
         <f ca="1">IF($X$10 &lt; F4, 1, 0)</f>
@@ -7218,16 +8438,16 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J9">
         <v>20</v>
       </c>
       <c r="K9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -7242,14 +8462,14 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
       <c r="U9">
         <f ca="1">RANDBETWEEN(1, 100)</f>
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="V9">
         <f>((1-(ABS(P5-Q5)))/(P5+Q5) * ((P5+Q5)/2))</f>
@@ -7257,7 +8477,7 @@
       </c>
       <c r="W9">
         <f ca="1">IF($W$10 &lt; AD9, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X9">
         <f ca="1">IF($X$10 &lt; F5, 1, 0)</f>
@@ -7293,13 +8513,13 @@
         <v>20</v>
       </c>
       <c r="I10">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J10">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K10">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -7314,22 +8534,22 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="S10">
         <f ca="1">RANDBETWEEN(1, 100)</f>
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="W10">
         <f ca="1">RANDBETWEEN(1, 100)</f>
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="X10">
         <f ca="1">RANDBETWEEN(1, 100)</f>
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AF10" t="s">
         <v>167</v>
@@ -7355,16 +8575,16 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I11">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J11">
         <v>20</v>
       </c>
       <c r="K11">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -7379,10 +8599,10 @@
         <v>0</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
@@ -7405,16 +8625,16 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I12">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J12">
         <v>20</v>
       </c>
       <c r="K12">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -7429,7 +8649,7 @@
         <v>0</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -7440,7 +8660,7 @@
         <v>95</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -7455,16 +8675,16 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I13">
         <v>20</v>
       </c>
       <c r="J13">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K13">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -7479,10 +8699,13 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13">
         <v>0</v>
+      </c>
+      <c r="S13" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
@@ -7505,13 +8728,13 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I14">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J14">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K14">
         <v>20</v>
@@ -7532,7 +8755,11 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <f ca="1">RANDBETWEEN(1, 20)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
@@ -7564,7 +8791,7 @@
         <v>20</v>
       </c>
       <c r="K15">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -7582,7 +8809,7 @@
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
@@ -7602,16 +8829,16 @@
         <v>10</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H16">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I16">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J16">
-        <v>20</v>
+        <v>16.5</v>
       </c>
       <c r="K16">
         <v>20</v>
@@ -7632,7 +8859,7 @@
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
@@ -7640,7 +8867,7 @@
         <v>99</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -7655,13 +8882,13 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>20</v>
+        <v>11.25</v>
       </c>
       <c r="I17">
-        <v>20</v>
+        <v>11.25</v>
       </c>
       <c r="J17">
-        <v>20</v>
+        <v>11.25</v>
       </c>
       <c r="K17">
         <v>20</v>
@@ -7708,13 +8935,13 @@
         <v>20</v>
       </c>
       <c r="I18">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J18">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K18">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -7729,7 +8956,7 @@
         <v>0</v>
       </c>
       <c r="P18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -8055,16 +9282,16 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I25">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J25">
         <v>20</v>
       </c>
       <c r="K25">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -8079,7 +9306,7 @@
         <v>0</v>
       </c>
       <c r="P25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q25">
         <v>0</v>
@@ -11245,7 +12472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH232"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
@@ -20634,7 +21861,7 @@
   <dimension ref="V3:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AZ32" sqref="AZ32"/>
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20657,7 +21884,7 @@
       </c>
       <c r="X4">
         <f>ROUND(SUM((W4/$W$8)*100), 3)</f>
-        <v>43.103000000000002</v>
+        <v>39.683</v>
       </c>
       <c r="Y4" t="s">
         <v>67</v>
@@ -20668,11 +21895,11 @@
         <v>62</v>
       </c>
       <c r="W5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="X5">
         <f t="shared" ref="X5:X7" si="0">ROUND(SUM((W5/$W$8)*100), 3)</f>
-        <v>31.033999999999999</v>
+        <v>30.158999999999999</v>
       </c>
       <c r="Y5" t="s">
         <v>67</v>
@@ -20683,11 +21910,11 @@
         <v>63</v>
       </c>
       <c r="W6">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="X6">
         <f t="shared" si="0"/>
-        <v>12.069000000000001</v>
+        <v>17.46</v>
       </c>
       <c r="Y6" t="s">
         <v>67</v>
@@ -20702,7 +21929,7 @@
       </c>
       <c r="X7">
         <f t="shared" si="0"/>
-        <v>13.792999999999999</v>
+        <v>12.698</v>
       </c>
       <c r="Y7" t="s">
         <v>67</v>
@@ -20714,11 +21941,11 @@
       </c>
       <c r="W8" s="14">
         <f>SUM(W4:W7)</f>
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="X8" s="14">
         <f>SUM(X4:X7)</f>
-        <v>99.998999999999995</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="22:25" x14ac:dyDescent="0.25">
@@ -20768,7 +21995,7 @@
       </c>
       <c r="W16">
         <f t="shared" si="1"/>
-        <v>29.005882352941182</v>
+        <v>0</v>
       </c>
       <c r="X16" t="s">
         <v>67</v>
@@ -20780,7 +22007,7 @@
       </c>
       <c r="W17">
         <f t="shared" si="1"/>
-        <v>18.864705882352951</v>
+        <v>25.305882352941179</v>
       </c>
       <c r="X17" t="s">
         <v>67</v>
@@ -21218,6 +22445,1591 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:Q88"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AR34" sqref="AR34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="18" width="7.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>188</v>
+      </c>
+      <c r="H2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I2" t="s">
+        <v>191</v>
+      </c>
+      <c r="J2" t="s">
+        <v>189</v>
+      </c>
+      <c r="M2" t="s">
+        <v>204</v>
+      </c>
+      <c r="P2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3">
+        <f ca="1">COUNTIFS($C$9:$C$88, 1, $D$9:$D$88, 1)</f>
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <f ca="1">COUNTIFS($C$9:$C$88, 2, $D$9:$D$88, 1)</f>
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <f ca="1">COUNTIFS($C$9:$C$88, 3, $D$9:$D$88, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <f ca="1">COUNTIFS($C$9:$C$88, 4, $D$9:$D$88, 1)</f>
+        <v>8</v>
+      </c>
+      <c r="K3" s="14">
+        <f ca="1">SUM(G3:J3)</f>
+        <v>19</v>
+      </c>
+      <c r="M3">
+        <v>10</v>
+      </c>
+      <c r="P3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4">
+        <f ca="1">COUNTIFS($C$9:$C$88, 1, $D$9:$D$88, 2)</f>
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <f ca="1">COUNTIFS($C$9:$C$88, 2, $D$9:$D$88, 2)</f>
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <f ca="1">COUNTIFS($C$9:$C$88, 3, $D$9:$D$88, 2)</f>
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <f ca="1">COUNTIFS($C$9:$C$88, 4, $D$9:$D$88, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="K4" s="14">
+        <f t="shared" ref="K4:K6" ca="1" si="0">SUM(G4:J4)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5">
+        <f ca="1">COUNTIFS($C$9:$C$88, 1, $D$9:$D$88, 3)</f>
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <f ca="1">COUNTIFS($C$9:$C$88, 2, $D$9:$D$88, 3)</f>
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <f ca="1">COUNTIFS($C$9:$C$88, 3, $D$9:$D$88, 3)</f>
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <f ca="1">COUNTIFS($C$9:$C$88, 4, $D$9:$D$88, 3)</f>
+        <v>7</v>
+      </c>
+      <c r="K5" s="14">
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="P5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6">
+        <f ca="1">COUNTIFS($C$9:$C$88, 1, $D$9:$D$88, 4)</f>
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <f ca="1">COUNTIFS($C$9:$C$88, 2, $D$9:$D$88, 4)</f>
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <f ca="1">COUNTIFS($C$9:$C$88, 3, $D$9:$D$88, 4)</f>
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <f ca="1">COUNTIFS($C$9:$C$88, 4, $D$9:$D$88, 4)</f>
+        <v>5</v>
+      </c>
+      <c r="K6" s="14">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="P6">
+        <f ca="1">G15/P3</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="G7" s="14">
+        <f ca="1">SUM(G3:G6)</f>
+        <v>21</v>
+      </c>
+      <c r="H7" s="14">
+        <f t="shared" ref="H7:J7" ca="1" si="1">SUM(H3:H6)</f>
+        <v>16</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" ca="1" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" ca="1" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f ca="1">RANDBETWEEN(1, 4)</f>
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <f ca="1">RANDBETWEEN(1, 4)</f>
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>203</v>
+      </c>
+      <c r="N9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:D41" ca="1" si="2">RANDBETWEEN(1, 4)</f>
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" t="s">
+        <v>202</v>
+      </c>
+      <c r="K10" t="s">
+        <v>206</v>
+      </c>
+      <c r="L10" t="s">
+        <v>207</v>
+      </c>
+      <c r="N10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>188</v>
+      </c>
+      <c r="G11">
+        <f ca="1">COUNTIF(C9:C88, 1)</f>
+        <v>21</v>
+      </c>
+      <c r="H11">
+        <f ca="1">ABS(G11-$G$16)</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <f ca="1">$M$3-$H11</f>
+        <v>9</v>
+      </c>
+      <c r="K11" s="1">
+        <f ca="1">MAX(G11:G14)</f>
+        <v>26</v>
+      </c>
+      <c r="L11" s="1">
+        <f ca="1">$M$3-$H11</f>
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <f ca="1">MAX(G3:J6)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>190</v>
+      </c>
+      <c r="G12">
+        <f ca="1">COUNTIF(C9:C88, 2)</f>
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <f ca="1">ABS(G12-$G$16)</f>
+        <v>4</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" ref="I12:I14" ca="1" si="3">$M$3-$H12</f>
+        <v>6</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" ref="L12:L14" ca="1" si="4">$M$3-$H12</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>191</v>
+      </c>
+      <c r="G13">
+        <f ca="1">COUNTIF(C9:C88, 3)</f>
+        <v>17</v>
+      </c>
+      <c r="H13">
+        <f ca="1">ABS(G13-$G$16)</f>
+        <v>3</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>189</v>
+      </c>
+      <c r="G14">
+        <f ca="1">COUNTIF(C9:C88, 4)</f>
+        <v>26</v>
+      </c>
+      <c r="H14">
+        <f ca="1">ABS(G14-$G$16)</f>
+        <v>6</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="L14" s="1">
+        <f ca="1">$M$3-$H14</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="16">
+        <f ca="1">SUM(G11:G14)</f>
+        <v>80</v>
+      </c>
+      <c r="H15" s="16">
+        <f ca="1">SUM(H11:H14)</f>
+        <v>14</v>
+      </c>
+      <c r="I15" s="17">
+        <f ca="1">SUM(I11:I14)</f>
+        <v>26</v>
+      </c>
+      <c r="L15" s="17">
+        <f ca="1">SUM(L11:L14)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="G16">
+        <f ca="1">AVERAGE(G11:G14)</f>
+        <v>20</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18">
+        <f ca="1">COUNTIF(D9:D88, 1)</f>
+        <v>19</v>
+      </c>
+      <c r="H18">
+        <f ca="1">ABS(G18-$G$23)</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <f ca="1">$M$3-$H18</f>
+        <v>9</v>
+      </c>
+      <c r="K18" s="1">
+        <f ca="1">$M$3-$H18</f>
+        <v>9</v>
+      </c>
+      <c r="L18" s="1">
+        <f ca="1">MAX(G18:G21)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19">
+        <f ca="1">COUNTIF(D9:D88, 2)</f>
+        <v>19</v>
+      </c>
+      <c r="H19">
+        <f ca="1">ABS(G19-$G$23)</f>
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" ref="I19:K21" ca="1" si="5">$M$3-$H19</f>
+        <v>9</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20">
+        <f ca="1">COUNTIF(D9:D88, 3)</f>
+        <v>23</v>
+      </c>
+      <c r="H20">
+        <f ca="1">ABS(G20-$G$23)</f>
+        <v>3</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21">
+        <f ca="1">COUNTIF(D9:D88, 4)</f>
+        <v>19</v>
+      </c>
+      <c r="H21">
+        <f ca="1">ABS(G21-$G$23)</f>
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <f ca="1">$M$3-$H21</f>
+        <v>9</v>
+      </c>
+      <c r="K21" s="1">
+        <f ca="1">$M$3-$H21</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>14</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="16">
+        <f ca="1">SUM(G18:G21)</f>
+        <v>80</v>
+      </c>
+      <c r="H22" s="16">
+        <f ca="1">SUM(H18:H21)</f>
+        <v>6</v>
+      </c>
+      <c r="I22" s="17">
+        <f ca="1">SUM(I18:I21)</f>
+        <v>34</v>
+      </c>
+      <c r="K22" s="17">
+        <f ca="1">SUM(K18:K21)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>15</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="G23">
+        <f ca="1">AVERAGE(G18:G21)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>17</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1">
+        <f ca="1">SUM(I15, I22)</f>
+        <v>60</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1">
+        <f ca="1">SUM(K11,K22)</f>
+        <v>60</v>
+      </c>
+      <c r="L25" s="1">
+        <f ca="1">SUM(L15, L18)</f>
+        <v>49</v>
+      </c>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1">
+        <f ca="1">N11</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>18</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>19</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>21</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>22</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>23</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>25</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>26</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>27</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>28</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>29</v>
+      </c>
+      <c r="C37">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>30</v>
+      </c>
+      <c r="C38">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>31</v>
+      </c>
+      <c r="C39">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>32</v>
+      </c>
+      <c r="C40">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>33</v>
+      </c>
+      <c r="C41">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>34</v>
+      </c>
+      <c r="C42">
+        <f t="shared" ref="C42:D88" ca="1" si="6">RANDBETWEEN(1, 4)</f>
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>35</v>
+      </c>
+      <c r="C43">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>36</v>
+      </c>
+      <c r="C44">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>37</v>
+      </c>
+      <c r="C45">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>38</v>
+      </c>
+      <c r="C46">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>39</v>
+      </c>
+      <c r="C47">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>40</v>
+      </c>
+      <c r="C48">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>41</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D49">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>42</v>
+      </c>
+      <c r="C50">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>43</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>44</v>
+      </c>
+      <c r="C52">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D52">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>45</v>
+      </c>
+      <c r="C53">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D53">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>46</v>
+      </c>
+      <c r="C54">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D54">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>47</v>
+      </c>
+      <c r="C55">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>48</v>
+      </c>
+      <c r="C56">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D56">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>49</v>
+      </c>
+      <c r="C57">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>50</v>
+      </c>
+      <c r="C58">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D58">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>51</v>
+      </c>
+      <c r="C59">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>52</v>
+      </c>
+      <c r="C60">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>53</v>
+      </c>
+      <c r="C61">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>54</v>
+      </c>
+      <c r="C62">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>55</v>
+      </c>
+      <c r="C63">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>56</v>
+      </c>
+      <c r="C64">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>57</v>
+      </c>
+      <c r="C65">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D65">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>58</v>
+      </c>
+      <c r="C66">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D66">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>59</v>
+      </c>
+      <c r="C67">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>60</v>
+      </c>
+      <c r="C68">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D68">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>61</v>
+      </c>
+      <c r="C69">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>62</v>
+      </c>
+      <c r="C70">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D70">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>63</v>
+      </c>
+      <c r="C71">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>64</v>
+      </c>
+      <c r="C72">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>65</v>
+      </c>
+      <c r="C73">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D73">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>66</v>
+      </c>
+      <c r="C74">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D74">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>67</v>
+      </c>
+      <c r="C75">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>68</v>
+      </c>
+      <c r="C76">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D76">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>69</v>
+      </c>
+      <c r="C77">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D77">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>70</v>
+      </c>
+      <c r="C78">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D78">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>71</v>
+      </c>
+      <c r="C79">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D79">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>72</v>
+      </c>
+      <c r="C80">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D80">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>73</v>
+      </c>
+      <c r="C81">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>74</v>
+      </c>
+      <c r="C82">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>75</v>
+      </c>
+      <c r="C83">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>76</v>
+      </c>
+      <c r="C84">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>77</v>
+      </c>
+      <c r="C85">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D85">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>78</v>
+      </c>
+      <c r="C86">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="D86">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>79</v>
+      </c>
+      <c r="C87">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D87">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>80</v>
+      </c>
+      <c r="C88">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="D88">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G3:J6">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G14">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3FA1AA93-3C97-41E5-8075-541A805268FE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18:G21">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F11C508F-C137-42F7-AA0B-4593FC9A5AC9}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3FA1AA93-3C97-41E5-8075-541A805268FE}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G11:G14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F11C508F-C137-42F7-AA0B-4593FC9A5AC9}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G18:G21</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21231,7 +24043,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AX40"/>
   <sheetViews>
@@ -23256,7 +26068,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:C15"/>
   <sheetViews>

</xml_diff>